<commit_message>
Worked more of bear island drill
</commit_message>
<xml_diff>
--- a/ExcelEsport/FMWC_Examples/Bear Island - Harry Seiders - My Work.xlsx
+++ b/ExcelEsport/FMWC_Examples/Bear Island - Harry Seiders - My Work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\ExcelEsport\FMWC_Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A7F6DC-1BBE-4B6C-B57B-85EEACF295E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54C62F7-FEE1-4731-90A3-8B58A205842F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{114A3ACC-2F61-4F50-A5CF-63A86B2334B2}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="209">
   <si>
     <t>Bear Island</t>
   </si>
@@ -763,6 +763,12 @@
       </rPr>
       <t xml:space="preserve"> can be added to any of the baskets for an additional fee of $40.00</t>
     </r>
+  </si>
+  <si>
+    <t>Basket, Picnic Blanket, Paper Plates, Cups, Napkins, Utensils</t>
+  </si>
+  <si>
+    <t>Profit</t>
   </si>
 </sst>
 </file>
@@ -1934,7 +1940,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2324,6 +2330,33 @@
     <xf numFmtId="0" fontId="28" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2370,7 +2403,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>324825</xdr:rowOff>
+      <xdr:rowOff>321015</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2412,9 +2445,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>587795</xdr:colOff>
+      <xdr:colOff>591605</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>359004</xdr:rowOff>
+      <xdr:rowOff>362814</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2876,8 +2909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1BDF3C-7CF1-4670-8742-2CB86BCAA1B5}">
   <dimension ref="A1:AV222"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C53" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2896,8 +2929,8 @@
     <col min="12" max="12" width="7" style="1" customWidth="1"/>
     <col min="13" max="13" width="31" style="1" customWidth="1"/>
     <col min="14" max="14" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="4.88671875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="28.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.6640625" style="1" customWidth="1"/>
+    <col min="16" max="17" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7" style="1" customWidth="1"/>
     <col min="19" max="28" width="4.88671875" style="1" customWidth="1"/>
     <col min="29" max="48" width="4.5546875" style="1" customWidth="1"/>
@@ -3170,6 +3203,9 @@
       <c r="L12" s="80">
         <v>9</v>
       </c>
+      <c r="N12" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
       <c r="AJ12" s="6"/>
@@ -3199,6 +3235,14 @@
       </c>
       <c r="L13" s="81">
         <v>15</v>
+      </c>
+      <c r="N13" s="1" t="str" cm="1">
+        <f t="array" ref="N13:N18">TRIM(_xlfn.TEXTSPLIT(N12,,","))</f>
+        <v>Basket</v>
+      </c>
+      <c r="O13" s="1">
+        <f>_xlfn.XLOOKUP(N13,$K$12:$K$36,$L$12:$L$36)</f>
+        <v>75</v>
       </c>
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
@@ -3240,6 +3284,13 @@
       <c r="L14" s="81">
         <v>6</v>
       </c>
+      <c r="N14" s="1" t="str">
+        <v>Picnic Blanket</v>
+      </c>
+      <c r="O14" s="1">
+        <f>_xlfn.XLOOKUP(N14,$K$12:$K$36,$L$12:$L$36)</f>
+        <v>20</v>
+      </c>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
@@ -3280,6 +3331,13 @@
       <c r="L15" s="81">
         <v>7</v>
       </c>
+      <c r="N15" s="1" t="str">
+        <v>Paper Plates</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" ref="O14:O18" si="0">_xlfn.XLOOKUP(N15,$K$12:$K$36,$L$12:$L$36)</f>
+        <v>3</v>
+      </c>
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
@@ -3313,6 +3371,13 @@
       <c r="L16" s="81">
         <v>75</v>
       </c>
+      <c r="N16" s="1" t="str">
+        <v>Cups</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
@@ -3346,6 +3411,13 @@
       <c r="L17" s="81">
         <v>7</v>
       </c>
+      <c r="N17" s="1" t="str">
+        <v>Napkins</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="AE17" s="3"/>
       <c r="AF17" s="3"/>
       <c r="AG17" s="3"/>
@@ -3380,6 +3452,13 @@
         <v>5</v>
       </c>
       <c r="M18" s="3"/>
+      <c r="N18" s="1" t="str">
+        <v>Utensils</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
@@ -3416,7 +3495,10 @@
         <v>5</v>
       </c>
       <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="O19" s="1">
+        <f>SUM(O13:O18)</f>
+        <v>101</v>
+      </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
@@ -3466,6 +3548,13 @@
         <v>12</v>
       </c>
       <c r="M21" s="3"/>
+      <c r="N21" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="1" cm="1">
+        <f t="array" ref="O21">SUM(_xlfn.XLOOKUP(TRIM(_xlfn.TEXTSPLIT(F23,",")),$K$12:$K$36,$L$12:$L$36))+$O$19</f>
+        <v>118</v>
+      </c>
       <c r="AN21" s="3"/>
       <c r="AO21" s="3"/>
       <c r="AP21" s="3"/>
@@ -3499,6 +3588,13 @@
         <v>25</v>
       </c>
       <c r="M22" s="3"/>
+      <c r="N22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O22" s="1" cm="1">
+        <f t="array" ref="O22">SUM(_xlfn.XLOOKUP(TRIM(_xlfn.TEXTSPLIT(F24,",")),$K$12:$K$36,$L$12:$L$36))+$O$19</f>
+        <v>121</v>
+      </c>
       <c r="AN22" s="3"/>
       <c r="AO22" s="3"/>
       <c r="AP22" s="3"/>
@@ -3517,12 +3613,14 @@
       <c r="D23" s="46">
         <v>140</v>
       </c>
-      <c r="E23" s="50" t="s">
+      <c r="E23" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="153" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="84"/>
+      <c r="G23" s="147"/>
+      <c r="H23" s="148"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23" s="58" t="s">
@@ -3532,6 +3630,13 @@
         <v>7</v>
       </c>
       <c r="M23" s="3"/>
+      <c r="N23" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="1" cm="1">
+        <f t="array" ref="O23">SUM(_xlfn.XLOOKUP(TRIM(_xlfn.TEXTSPLIT(F25,",")),$K$12:$K$36,$L$12:$L$36))+$O$19</f>
+        <v>125</v>
+      </c>
       <c r="AN23" s="3"/>
       <c r="AO23" s="3"/>
       <c r="AP23" s="3"/>
@@ -3550,12 +3655,14 @@
       <c r="D24" s="29">
         <v>150</v>
       </c>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="85"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="86"/>
+      <c r="G24" s="149"/>
+      <c r="H24" s="150"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24" s="58" t="s">
@@ -3565,6 +3672,13 @@
         <v>22</v>
       </c>
       <c r="M24" s="3"/>
+      <c r="N24" t="s">
+        <v>31</v>
+      </c>
+      <c r="O24" s="1" cm="1">
+        <f t="array" ref="O24">SUM(_xlfn.XLOOKUP(TRIM(_xlfn.TEXTSPLIT(F26,",")),$K$12:$K$36,$L$12:$L$36))+$O$19</f>
+        <v>132</v>
+      </c>
       <c r="AN24" s="3"/>
       <c r="AO24" s="3"/>
       <c r="AP24" s="3"/>
@@ -3583,12 +3697,14 @@
       <c r="D25" s="29">
         <v>155</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="154" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="86"/>
+      <c r="G25" s="149"/>
+      <c r="H25" s="150"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25" s="58" t="s">
@@ -3598,6 +3714,13 @@
         <v>10</v>
       </c>
       <c r="M25" s="3"/>
+      <c r="N25" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25" s="1" cm="1">
+        <f t="array" ref="O25">SUM(_xlfn.XLOOKUP(TRIM(_xlfn.TEXTSPLIT(F27,",")),$K$12:$K$36,$L$12:$L$36))+$O$19</f>
+        <v>117</v>
+      </c>
       <c r="AJ25" s="3"/>
       <c r="AK25" s="3"/>
       <c r="AM25" s="3"/>
@@ -3619,12 +3742,14 @@
       <c r="D26" s="29">
         <v>160</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="154" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="85"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="86"/>
+      <c r="G26" s="149"/>
+      <c r="H26" s="150"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26" s="58" t="s">
@@ -3634,6 +3759,13 @@
         <v>1</v>
       </c>
       <c r="M26" s="3"/>
+      <c r="N26" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" s="1" cm="1">
+        <f t="array" ref="O26">SUM(_xlfn.XLOOKUP(TRIM(_xlfn.TEXTSPLIT(F28,",")),$K$12:$K$36,$L$12:$L$36))+$O$19</f>
+        <v>141</v>
+      </c>
       <c r="AS26" s="4"/>
       <c r="AT26" s="4"/>
       <c r="AU26" s="4"/>
@@ -3647,12 +3779,14 @@
       <c r="D27" s="29">
         <v>145</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="154" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="85"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="86"/>
+      <c r="G27" s="149"/>
+      <c r="H27" s="150"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27" s="58" t="s">
@@ -3662,6 +3796,14 @@
         <v>3</v>
       </c>
       <c r="M27" s="3"/>
+      <c r="N27" t="str" cm="1">
+        <f t="array" ref="N27:N32">N21:N26&amp;" with Wine Added"</f>
+        <v>Berry Basket with Wine Added</v>
+      </c>
+      <c r="O27" s="1" cm="1">
+        <f t="array" ref="O27:O32">18+O21:O26</f>
+        <v>136</v>
+      </c>
       <c r="AS27" s="4"/>
       <c r="AT27" s="4"/>
       <c r="AU27" s="4"/>
@@ -3675,12 +3817,14 @@
       <c r="D28" s="54">
         <v>170</v>
       </c>
-      <c r="E28" s="55" t="s">
+      <c r="E28" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="155" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="88"/>
+      <c r="G28" s="151"/>
+      <c r="H28" s="152"/>
       <c r="I28" s="45"/>
       <c r="J28" s="45"/>
       <c r="K28" s="58" t="s">
@@ -3690,6 +3834,12 @@
         <v>8</v>
       </c>
       <c r="M28" s="3"/>
+      <c r="N28" t="str">
+        <v>Cheesy Basket with Wine Added</v>
+      </c>
+      <c r="O28" s="1">
+        <v>139</v>
+      </c>
       <c r="AS28" s="4"/>
       <c r="AT28" s="4"/>
       <c r="AU28" s="4"/>
@@ -3712,6 +3862,12 @@
         <v>20</v>
       </c>
       <c r="M29" s="3"/>
+      <c r="N29" t="str">
+        <v>Fruity Basket with Wine Added</v>
+      </c>
+      <c r="O29" s="1">
+        <v>143</v>
+      </c>
       <c r="AS29" s="4"/>
       <c r="AT29" s="4"/>
       <c r="AU29" s="4"/>
@@ -3736,6 +3892,12 @@
         <v>6</v>
       </c>
       <c r="M30" s="3"/>
+      <c r="N30" t="str">
+        <v>Hungry Basket with Wine Added</v>
+      </c>
+      <c r="O30" s="1">
+        <v>150</v>
+      </c>
       <c r="AS30" s="4"/>
       <c r="AT30" s="4"/>
       <c r="AU30" s="4"/>
@@ -3758,6 +3920,12 @@
         <v>4</v>
       </c>
       <c r="M31" s="3"/>
+      <c r="N31" t="str">
+        <v>Snack Basket with Wine Added</v>
+      </c>
+      <c r="O31" s="1">
+        <v>135</v>
+      </c>
       <c r="AS31" s="4"/>
       <c r="AT31" s="4"/>
       <c r="AU31" s="4"/>
@@ -3788,6 +3956,12 @@
         <v>3</v>
       </c>
       <c r="M32" s="3"/>
+      <c r="N32" t="str">
+        <v>Bucket Basket with Wine Added</v>
+      </c>
+      <c r="O32" s="1">
+        <v>159</v>
+      </c>
       <c r="AS32" s="4"/>
       <c r="AT32" s="4"/>
       <c r="AU32" s="4"/>
@@ -4270,7 +4444,7 @@
     <row r="50" spans="2:48" ht="14.85" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="K50" s="117">
         <f>SUMPRODUCT(D:D,F:F)</f>
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="AK50" s="4"/>
       <c r="AL50" s="4"/>
@@ -4470,8 +4644,12 @@
       <c r="N57" t="s">
         <v>19</v>
       </c>
-      <c r="O57"/>
-      <c r="P57"/>
+      <c r="O57" t="s">
+        <v>4</v>
+      </c>
+      <c r="P57" t="s">
+        <v>208</v>
+      </c>
       <c r="Q57"/>
       <c r="R57"/>
       <c r="AJ57" s="4"/>
@@ -4522,8 +4700,14 @@
       <c r="N58">
         <v>140</v>
       </c>
-      <c r="O58"/>
-      <c r="P58"/>
+      <c r="O58" s="1" cm="1">
+        <f t="array" ref="O58:O69">O21:O32</f>
+        <v>118</v>
+      </c>
+      <c r="P58" cm="1">
+        <f t="array" ref="P58:P69">N58:N69-O58:O69</f>
+        <v>22</v>
+      </c>
       <c r="Q58"/>
       <c r="R58"/>
       <c r="AJ58" s="4"/>
@@ -4573,8 +4757,12 @@
       <c r="N59">
         <v>150</v>
       </c>
-      <c r="O59"/>
-      <c r="P59"/>
+      <c r="O59" s="1">
+        <v>121</v>
+      </c>
+      <c r="P59">
+        <v>29</v>
+      </c>
       <c r="Q59"/>
       <c r="R59"/>
       <c r="AJ59" s="4"/>
@@ -4593,7 +4781,7 @@
     </row>
     <row r="60" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B60" s="17">
-        <f t="shared" ref="B60:B122" si="0">B59+1</f>
+        <f t="shared" ref="B60:B122" si="1">B59+1</f>
         <v>4</v>
       </c>
       <c r="C60" s="17">
@@ -4624,8 +4812,12 @@
       <c r="N60">
         <v>155</v>
       </c>
-      <c r="O60"/>
-      <c r="P60"/>
+      <c r="O60" s="1">
+        <v>125</v>
+      </c>
+      <c r="P60">
+        <v>30</v>
+      </c>
       <c r="Q60"/>
       <c r="R60"/>
       <c r="AJ60" s="4"/>
@@ -4644,7 +4836,7 @@
     </row>
     <row r="61" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B61" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C61" s="17">
@@ -4675,8 +4867,12 @@
       <c r="N61">
         <v>160</v>
       </c>
-      <c r="O61"/>
-      <c r="P61"/>
+      <c r="O61" s="1">
+        <v>132</v>
+      </c>
+      <c r="P61">
+        <v>28</v>
+      </c>
       <c r="Q61"/>
       <c r="R61"/>
       <c r="AJ61" s="4"/>
@@ -4695,7 +4891,7 @@
     </row>
     <row r="62" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B62" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C62" s="17">
@@ -4726,8 +4922,12 @@
       <c r="N62">
         <v>145</v>
       </c>
-      <c r="O62"/>
-      <c r="P62"/>
+      <c r="O62" s="1">
+        <v>117</v>
+      </c>
+      <c r="P62">
+        <v>28</v>
+      </c>
       <c r="Q62"/>
       <c r="R62"/>
       <c r="AJ62" s="4"/>
@@ -4746,7 +4946,7 @@
     </row>
     <row r="63" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B63" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C63" s="17">
@@ -4777,8 +4977,12 @@
       <c r="N63">
         <v>170</v>
       </c>
-      <c r="O63"/>
-      <c r="P63"/>
+      <c r="O63" s="1">
+        <v>141</v>
+      </c>
+      <c r="P63">
+        <v>29</v>
+      </c>
       <c r="Q63"/>
       <c r="R63"/>
       <c r="AJ63" s="4"/>
@@ -4797,7 +5001,7 @@
     </row>
     <row r="64" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B64" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C64" s="17">
@@ -4829,6 +5033,12 @@
       <c r="N64" s="1" cm="1">
         <f t="array" ref="N64:N69">N58:N63+40</f>
         <v>180</v>
+      </c>
+      <c r="O64" s="1">
+        <v>136</v>
+      </c>
+      <c r="P64" s="1">
+        <v>44</v>
       </c>
       <c r="AK64" s="4"/>
       <c r="AL64" s="4"/>
@@ -4845,7 +5055,7 @@
     </row>
     <row r="65" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B65" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C65" s="17">
@@ -4875,6 +5085,12 @@
       </c>
       <c r="N65" s="1">
         <v>190</v>
+      </c>
+      <c r="O65" s="1">
+        <v>139</v>
+      </c>
+      <c r="P65" s="1">
+        <v>51</v>
       </c>
       <c r="AK65" s="4"/>
       <c r="AL65" s="4"/>
@@ -4891,7 +5107,7 @@
     </row>
     <row r="66" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B66" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C66" s="17">
@@ -4921,6 +5137,12 @@
       </c>
       <c r="N66" s="1">
         <v>195</v>
+      </c>
+      <c r="O66" s="1">
+        <v>143</v>
+      </c>
+      <c r="P66" s="1">
+        <v>52</v>
       </c>
       <c r="AK66" s="4"/>
       <c r="AL66" s="4"/>
@@ -4946,6 +5168,12 @@
       <c r="N67" s="1">
         <v>200</v>
       </c>
+      <c r="O67" s="1">
+        <v>150</v>
+      </c>
+      <c r="P67" s="1">
+        <v>50</v>
+      </c>
       <c r="AK67" s="4"/>
       <c r="AL67" s="4"/>
       <c r="AM67" s="4"/>
@@ -4983,6 +5211,12 @@
       <c r="N68" s="1">
         <v>185</v>
       </c>
+      <c r="O68" s="1">
+        <v>135</v>
+      </c>
+      <c r="P68" s="1">
+        <v>50</v>
+      </c>
       <c r="AK68" s="4"/>
       <c r="AL68" s="4"/>
       <c r="AM68" s="4"/>
@@ -5006,6 +5240,12 @@
       </c>
       <c r="N69" s="1">
         <v>210</v>
+      </c>
+      <c r="O69" s="1">
+        <v>159</v>
+      </c>
+      <c r="P69" s="1">
+        <v>51</v>
       </c>
       <c r="AK69" s="4"/>
       <c r="AL69" s="4"/>
@@ -5231,6 +5471,14 @@
       <c r="H79" s="25">
         <v>3</v>
       </c>
+      <c r="K79" s="1" cm="1">
+        <f t="array" ref="K79:K100">_xlfn.XLOOKUP(G79:G100,$M$58:$M$69,$N$58:$N$69)*H79:H100</f>
+        <v>600</v>
+      </c>
+      <c r="M79" s="1">
+        <f>3*P58</f>
+        <v>66</v>
+      </c>
       <c r="AJ79" s="4"/>
       <c r="AK79" s="4"/>
       <c r="AL79" s="4"/>
@@ -5250,6 +5498,9 @@
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
+      <c r="K80" s="1" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="AJ80" s="4"/>
       <c r="AK80" s="4"/>
       <c r="AL80" s="4"/>
@@ -5274,16 +5525,25 @@
       <c r="D81" s="18">
         <v>8</v>
       </c>
-      <c r="E81" s="19"/>
+      <c r="E81" s="19">
+        <v>176</v>
+      </c>
       <c r="F81" s="37">
         <f>IF(ISBLANK(E81),0,IF(E81=Answers!E81,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H81" s="25">
         <v>8</v>
+      </c>
+      <c r="I81" s="1" cm="1">
+        <f t="array" ref="I81">_xlfn.XLOOKUP(G81,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H81</f>
+        <v>176</v>
+      </c>
+      <c r="K81" s="1">
+        <v>1120</v>
       </c>
       <c r="AJ81" s="4"/>
       <c r="AK81" s="4"/>
@@ -5301,7 +5561,7 @@
     </row>
     <row r="82" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C82" s="17">
@@ -5310,16 +5570,25 @@
       <c r="D82" s="18">
         <v>8</v>
       </c>
-      <c r="E82" s="19"/>
+      <c r="E82" s="19">
+        <v>84</v>
+      </c>
       <c r="F82" s="37">
         <f>IF(ISBLANK(E82),0,IF(E82=Answers!E82,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" s="25" t="s">
         <v>31</v>
       </c>
       <c r="H82" s="25">
         <v>3</v>
+      </c>
+      <c r="I82" s="1" cm="1">
+        <f t="array" ref="I82">_xlfn.XLOOKUP(G82,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H82</f>
+        <v>84</v>
+      </c>
+      <c r="K82" s="1">
+        <v>480</v>
       </c>
       <c r="AJ82" s="4"/>
       <c r="AK82" s="4"/>
@@ -5337,7 +5606,7 @@
     </row>
     <row r="83" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="C83" s="17">
@@ -5346,16 +5615,25 @@
       <c r="D83" s="18">
         <v>8</v>
       </c>
-      <c r="E83" s="19"/>
+      <c r="E83" s="19">
+        <v>392</v>
+      </c>
       <c r="F83" s="37">
         <f>IF(ISBLANK(E83),0,IF(E83=Answers!E83,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83" s="25" t="s">
         <v>34</v>
       </c>
       <c r="H83" s="25">
         <v>14</v>
+      </c>
+      <c r="I83" s="1" cm="1">
+        <f t="array" ref="I83">_xlfn.XLOOKUP(G83,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H83</f>
+        <v>392</v>
+      </c>
+      <c r="K83" s="1">
+        <v>2030</v>
       </c>
       <c r="AJ83" s="4"/>
       <c r="AK83" s="4"/>
@@ -5373,7 +5651,7 @@
     </row>
     <row r="84" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C84" s="17">
@@ -5382,16 +5660,25 @@
       <c r="D84" s="18">
         <v>8</v>
       </c>
-      <c r="E84" s="19"/>
+      <c r="E84" s="19">
+        <v>306</v>
+      </c>
       <c r="F84" s="37">
         <f>IF(ISBLANK(E84),0,IF(E84=Answers!E84,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84" s="25" t="s">
         <v>82</v>
       </c>
       <c r="H84" s="25">
         <v>6</v>
+      </c>
+      <c r="I84" s="1" cm="1">
+        <f t="array" ref="I84">_xlfn.XLOOKUP(G84,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H84</f>
+        <v>306</v>
+      </c>
+      <c r="K84" s="1">
+        <v>1260</v>
       </c>
       <c r="AJ84" s="4"/>
       <c r="AK84" s="4"/>
@@ -5409,7 +5696,7 @@
     </row>
     <row r="85" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C85" s="17">
@@ -5418,16 +5705,25 @@
       <c r="D85" s="18">
         <v>8</v>
       </c>
-      <c r="E85" s="19"/>
+      <c r="E85" s="19">
+        <v>210</v>
+      </c>
       <c r="F85" s="37">
         <f>IF(ISBLANK(E85),0,IF(E85=Answers!E85,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85" s="25" t="s">
         <v>28</v>
       </c>
       <c r="H85" s="25">
         <v>7</v>
+      </c>
+      <c r="I85" s="1" cm="1">
+        <f t="array" ref="I85">_xlfn.XLOOKUP(G85,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H85</f>
+        <v>210</v>
+      </c>
+      <c r="K85" s="1">
+        <v>1085</v>
       </c>
       <c r="AJ85" s="4"/>
       <c r="AK85" s="4"/>
@@ -5445,7 +5741,7 @@
     </row>
     <row r="86" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C86" s="17">
@@ -5454,16 +5750,25 @@
       <c r="D86" s="18">
         <v>8</v>
       </c>
-      <c r="E86" s="19"/>
+      <c r="E86" s="19">
+        <v>408</v>
+      </c>
       <c r="F86" s="37">
         <f>IF(ISBLANK(E86),0,IF(E86=Answers!E86,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86" s="25" t="s">
         <v>83</v>
       </c>
       <c r="H86" s="25">
         <v>8</v>
+      </c>
+      <c r="I86" s="1" cm="1">
+        <f t="array" ref="I86">_xlfn.XLOOKUP(G86,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H86</f>
+        <v>408</v>
+      </c>
+      <c r="K86" s="1">
+        <v>1520</v>
       </c>
       <c r="AJ86" s="4"/>
       <c r="AK86" s="4"/>
@@ -5481,7 +5786,7 @@
     </row>
     <row r="87" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C87" s="17">
@@ -5490,16 +5795,25 @@
       <c r="D87" s="18">
         <v>8</v>
       </c>
-      <c r="E87" s="19"/>
+      <c r="E87" s="19">
+        <v>196</v>
+      </c>
       <c r="F87" s="37">
         <f>IF(ISBLANK(E87),0,IF(E87=Answers!E87,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G87" s="25" t="s">
         <v>34</v>
       </c>
       <c r="H87" s="25">
         <v>7</v>
+      </c>
+      <c r="I87" s="1" cm="1">
+        <f t="array" ref="I87">_xlfn.XLOOKUP(G87,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H87</f>
+        <v>196</v>
+      </c>
+      <c r="K87" s="1">
+        <v>1015</v>
       </c>
       <c r="AJ87" s="4"/>
       <c r="AK87" s="4"/>
@@ -5517,7 +5831,7 @@
     </row>
     <row r="88" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C88" s="17">
@@ -5526,16 +5840,25 @@
       <c r="D88" s="18">
         <v>8</v>
       </c>
-      <c r="E88" s="19"/>
+      <c r="E88" s="19">
+        <v>261</v>
+      </c>
       <c r="F88" s="37">
         <f>IF(ISBLANK(E88),0,IF(E88=Answers!E88,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G88" s="25" t="s">
         <v>37</v>
       </c>
       <c r="H88" s="25">
         <v>9</v>
+      </c>
+      <c r="I88" s="1" cm="1">
+        <f t="array" ref="I88">_xlfn.XLOOKUP(G88,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H88</f>
+        <v>261</v>
+      </c>
+      <c r="K88" s="1">
+        <v>1530</v>
       </c>
       <c r="AJ88" s="4"/>
       <c r="AK88" s="4"/>
@@ -5553,7 +5876,7 @@
     </row>
     <row r="89" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C89" s="17">
@@ -5562,16 +5885,25 @@
       <c r="D89" s="18">
         <v>8</v>
       </c>
-      <c r="E89" s="19"/>
+      <c r="E89" s="19">
+        <v>468</v>
+      </c>
       <c r="F89" s="37">
         <f>IF(ISBLANK(E89),0,IF(E89=Answers!E89,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G89" s="25" t="s">
         <v>84</v>
       </c>
       <c r="H89" s="25">
         <v>9</v>
+      </c>
+      <c r="I89" s="1" cm="1">
+        <f t="array" ref="I89">_xlfn.XLOOKUP(G89,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H89</f>
+        <v>468</v>
+      </c>
+      <c r="K89" s="1">
+        <v>1755</v>
       </c>
       <c r="AJ89" s="4"/>
       <c r="AK89" s="4"/>
@@ -5589,7 +5921,7 @@
     </row>
     <row r="90" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C90" s="17">
@@ -5598,16 +5930,25 @@
       <c r="D90" s="18">
         <v>8</v>
       </c>
-      <c r="E90" s="19"/>
+      <c r="E90" s="19">
+        <v>357</v>
+      </c>
       <c r="F90" s="37">
         <f>IF(ISBLANK(E90),0,IF(E90=Answers!E90,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90" s="25" t="s">
         <v>83</v>
       </c>
       <c r="H90" s="25">
         <v>7</v>
+      </c>
+      <c r="I90" s="1" cm="1">
+        <f t="array" ref="I90">_xlfn.XLOOKUP(G90,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H90</f>
+        <v>357</v>
+      </c>
+      <c r="K90" s="1">
+        <v>1330</v>
       </c>
       <c r="AJ90" s="4"/>
       <c r="AK90" s="4"/>
@@ -5625,7 +5966,7 @@
     </row>
     <row r="91" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C91" s="17">
@@ -5634,16 +5975,25 @@
       <c r="D91" s="18">
         <v>8</v>
       </c>
-      <c r="E91" s="19"/>
+      <c r="E91" s="19">
+        <v>484</v>
+      </c>
       <c r="F91" s="37">
         <f>IF(ISBLANK(E91),0,IF(E91=Answers!E91,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91" s="25" t="s">
         <v>92</v>
       </c>
       <c r="H91" s="25">
         <v>11</v>
+      </c>
+      <c r="I91" s="1" cm="1">
+        <f t="array" ref="I91">_xlfn.XLOOKUP(G91,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H91</f>
+        <v>484</v>
+      </c>
+      <c r="K91" s="1">
+        <v>1980</v>
       </c>
       <c r="AJ91" s="4"/>
       <c r="AK91" s="4"/>
@@ -5661,7 +6011,7 @@
     </row>
     <row r="92" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C92" s="17">
@@ -5670,16 +6020,25 @@
       <c r="D92" s="18">
         <v>8</v>
       </c>
-      <c r="E92" s="19"/>
+      <c r="E92" s="19">
+        <v>800</v>
+      </c>
       <c r="F92" s="37">
         <f>IF(ISBLANK(E92),0,IF(E92=Answers!E92,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92" s="25" t="s">
         <v>81</v>
       </c>
       <c r="H92" s="25">
         <v>16</v>
+      </c>
+      <c r="I92" s="1" cm="1">
+        <f t="array" ref="I92">_xlfn.XLOOKUP(G92,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H92</f>
+        <v>800</v>
+      </c>
+      <c r="K92" s="1">
+        <v>3200</v>
       </c>
       <c r="AJ92" s="4"/>
       <c r="AK92" s="4"/>
@@ -5697,7 +6056,7 @@
     </row>
     <row r="93" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C93" s="17">
@@ -5706,16 +6065,25 @@
       <c r="D93" s="18">
         <v>8</v>
       </c>
-      <c r="E93" s="19"/>
+      <c r="E93" s="19">
+        <v>700</v>
+      </c>
       <c r="F93" s="37">
         <f>IF(ISBLANK(E93),0,IF(E93=Answers!E93,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G93" s="25" t="s">
         <v>93</v>
       </c>
       <c r="H93" s="25">
         <v>14</v>
+      </c>
+      <c r="I93" s="1" cm="1">
+        <f t="array" ref="I93">_xlfn.XLOOKUP(G93,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H93</f>
+        <v>700</v>
+      </c>
+      <c r="K93" s="1">
+        <v>2590</v>
       </c>
       <c r="AJ93" s="4"/>
       <c r="AK93" s="4"/>
@@ -5733,7 +6101,7 @@
     </row>
     <row r="94" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C94" s="17">
@@ -5742,16 +6110,25 @@
       <c r="D94" s="18">
         <v>8</v>
       </c>
-      <c r="E94" s="19"/>
+      <c r="E94" s="19">
+        <v>104</v>
+      </c>
       <c r="F94" s="37">
         <f>IF(ISBLANK(E94),0,IF(E94=Answers!E94,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94" s="25" t="s">
         <v>84</v>
       </c>
       <c r="H94" s="25">
         <v>2</v>
+      </c>
+      <c r="I94" s="1" cm="1">
+        <f t="array" ref="I94">_xlfn.XLOOKUP(G94,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H94</f>
+        <v>104</v>
+      </c>
+      <c r="K94" s="1">
+        <v>390</v>
       </c>
       <c r="AJ94" s="4"/>
       <c r="AK94" s="4"/>
@@ -5769,7 +6146,7 @@
     </row>
     <row r="95" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C95" s="17">
@@ -5778,16 +6155,25 @@
       <c r="D95" s="18">
         <v>8</v>
       </c>
-      <c r="E95" s="19"/>
+      <c r="E95" s="19">
+        <v>250</v>
+      </c>
       <c r="F95" s="37">
         <f>IF(ISBLANK(E95),0,IF(E95=Answers!E95,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95" s="25" t="s">
         <v>93</v>
       </c>
       <c r="H95" s="25">
         <v>5</v>
+      </c>
+      <c r="I95" s="1" cm="1">
+        <f t="array" ref="I95">_xlfn.XLOOKUP(G95,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H95</f>
+        <v>250</v>
+      </c>
+      <c r="K95" s="1">
+        <v>925</v>
       </c>
       <c r="AJ95" s="4"/>
       <c r="AK95" s="4"/>
@@ -5805,7 +6191,7 @@
     </row>
     <row r="96" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C96" s="17">
@@ -5814,16 +6200,25 @@
       <c r="D96" s="18">
         <v>8</v>
       </c>
-      <c r="E96" s="19"/>
+      <c r="E96" s="19">
+        <v>252</v>
+      </c>
       <c r="F96" s="37">
         <f>IF(ISBLANK(E96),0,IF(E96=Answers!E96,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G96" s="25" t="s">
         <v>31</v>
       </c>
       <c r="H96" s="25">
         <v>9</v>
+      </c>
+      <c r="I96" s="1" cm="1">
+        <f t="array" ref="I96">_xlfn.XLOOKUP(G96,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H96</f>
+        <v>252</v>
+      </c>
+      <c r="K96" s="1">
+        <v>1440</v>
       </c>
       <c r="AJ96" s="4"/>
       <c r="AK96" s="4"/>
@@ -5841,7 +6236,7 @@
     </row>
     <row r="97" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C97" s="17">
@@ -5850,16 +6245,25 @@
       <c r="D97" s="18">
         <v>8</v>
       </c>
-      <c r="E97" s="19"/>
+      <c r="E97" s="19">
+        <v>364</v>
+      </c>
       <c r="F97" s="37">
         <f>IF(ISBLANK(E97),0,IF(E97=Answers!E97,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G97" s="25" t="s">
         <v>34</v>
       </c>
       <c r="H97" s="25">
         <v>13</v>
+      </c>
+      <c r="I97" s="1" cm="1">
+        <f t="array" ref="I97">_xlfn.XLOOKUP(G97,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H97</f>
+        <v>364</v>
+      </c>
+      <c r="K97" s="1">
+        <v>1885</v>
       </c>
       <c r="AJ97" s="4"/>
       <c r="AK97" s="4"/>
@@ -5877,7 +6281,7 @@
     </row>
     <row r="98" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C98" s="17">
@@ -5886,16 +6290,25 @@
       <c r="D98" s="18">
         <v>8</v>
       </c>
-      <c r="E98" s="19"/>
+      <c r="E98" s="19">
+        <v>87</v>
+      </c>
       <c r="F98" s="37">
         <f>IF(ISBLANK(E98),0,IF(E98=Answers!E98,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98" s="25" t="s">
         <v>37</v>
       </c>
       <c r="H98" s="25">
         <v>3</v>
+      </c>
+      <c r="I98" s="1" cm="1">
+        <f t="array" ref="I98">_xlfn.XLOOKUP(G98,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H98</f>
+        <v>87</v>
+      </c>
+      <c r="K98" s="1">
+        <v>510</v>
       </c>
       <c r="AJ98" s="4"/>
       <c r="AK98" s="4"/>
@@ -5913,7 +6326,7 @@
     </row>
     <row r="99" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C99" s="17">
@@ -5922,16 +6335,25 @@
       <c r="D99" s="18">
         <v>8</v>
       </c>
-      <c r="E99" s="19"/>
+      <c r="E99" s="19">
+        <v>1092</v>
+      </c>
       <c r="F99" s="37">
         <f>IF(ISBLANK(E99),0,IF(E99=Answers!E99,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99" s="25" t="s">
         <v>84</v>
       </c>
       <c r="H99" s="25">
         <v>21</v>
+      </c>
+      <c r="I99" s="1" cm="1">
+        <f t="array" ref="I99">_xlfn.XLOOKUP(G99,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H99</f>
+        <v>1092</v>
+      </c>
+      <c r="K99" s="1">
+        <v>4095</v>
       </c>
       <c r="AJ99" s="4"/>
       <c r="AK99" s="4"/>
@@ -5949,7 +6371,7 @@
     </row>
     <row r="100" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C100" s="17">
@@ -5958,16 +6380,25 @@
       <c r="D100" s="18">
         <v>8</v>
       </c>
-      <c r="E100" s="19"/>
+      <c r="E100" s="19">
+        <v>1150</v>
+      </c>
       <c r="F100" s="37">
         <f>IF(ISBLANK(E100),0,IF(E100=Answers!E100,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100" s="25" t="s">
         <v>81</v>
       </c>
       <c r="H100" s="25">
         <v>23</v>
+      </c>
+      <c r="I100" s="1" cm="1">
+        <f t="array" ref="I100">_xlfn.XLOOKUP(G100,$M$58:$M$69,_xlfn.ANCHORARRAY($P$58))*H100</f>
+        <v>1150</v>
+      </c>
+      <c r="K100" s="1">
+        <v>4600</v>
       </c>
       <c r="AJ100" s="4"/>
       <c r="AK100" s="4"/>
@@ -6013,11 +6444,11 @@
       </c>
       <c r="E102" s="19">
         <f>SUM(E81:E100)</f>
-        <v>0</v>
+        <v>8141</v>
       </c>
       <c r="F102" s="37">
         <f>IF(ISBLANK(E102),0,IF(E102=Answers!E102,1,-1))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AK102" s="4"/>
       <c r="AL102" s="4"/>
@@ -6411,7 +6842,7 @@
     </row>
     <row r="116" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B116" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="C116" s="17">
@@ -6458,7 +6889,7 @@
     </row>
     <row r="117" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B117" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="C117" s="17">
@@ -6505,7 +6936,7 @@
     </row>
     <row r="118" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B118" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="C118" s="17">
@@ -6552,7 +6983,7 @@
     </row>
     <row r="119" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B119" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C119" s="17">
@@ -6599,7 +7030,7 @@
     </row>
     <row r="120" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B120" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C120" s="17">
@@ -6646,7 +7077,7 @@
     </row>
     <row r="121" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B121" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="C121" s="17">
@@ -6693,7 +7124,7 @@
     </row>
     <row r="122" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B122" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C122" s="17">
@@ -6740,7 +7171,7 @@
     </row>
     <row r="123" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B123" s="17">
-        <f t="shared" ref="B123:B188" si="1">B122+1</f>
+        <f t="shared" ref="B123:B188" si="2">B122+1</f>
         <v>39</v>
       </c>
       <c r="C123" s="17">
@@ -6787,7 +7218,7 @@
     </row>
     <row r="124" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B124" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="C124" s="17">
@@ -6834,7 +7265,7 @@
     </row>
     <row r="125" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B125" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="C125" s="17">
@@ -6881,7 +7312,7 @@
     </row>
     <row r="126" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B126" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="C126" s="17">
@@ -6928,7 +7359,7 @@
     </row>
     <row r="127" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B127" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="C127" s="17">
@@ -6975,7 +7406,7 @@
     </row>
     <row r="128" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B128" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="C128" s="17">
@@ -7022,7 +7453,7 @@
     </row>
     <row r="129" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B129" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="C129" s="17">
@@ -7069,7 +7500,7 @@
     </row>
     <row r="130" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B130" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="C130" s="17">
@@ -7116,7 +7547,7 @@
     </row>
     <row r="131" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B131" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="C131" s="17">
@@ -7163,7 +7594,7 @@
     </row>
     <row r="132" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B132" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="C132" s="17">
@@ -7210,7 +7641,7 @@
     </row>
     <row r="133" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B133" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="C133" s="17">
@@ -7257,7 +7688,7 @@
     </row>
     <row r="134" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B134" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="C134" s="17">
@@ -7680,7 +8111,7 @@
     </row>
     <row r="150" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B150" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="C150" s="17">
@@ -7718,7 +8149,7 @@
     </row>
     <row r="151" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B151" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
       <c r="C151" s="17">
@@ -7756,7 +8187,7 @@
     </row>
     <row r="152" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B152" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="C152" s="17">
@@ -7794,7 +8225,7 @@
     </row>
     <row r="153" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B153" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="C153" s="17">
@@ -7832,7 +8263,7 @@
     </row>
     <row r="154" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B154" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
       <c r="C154" s="17">
@@ -7870,7 +8301,7 @@
     </row>
     <row r="155" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B155" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="C155" s="17">
@@ -7908,7 +8339,7 @@
     </row>
     <row r="156" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B156" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="C156" s="17">
@@ -7946,7 +8377,7 @@
     </row>
     <row r="157" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B157" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="C157" s="17">
@@ -7984,7 +8415,7 @@
     </row>
     <row r="158" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B158" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="C158" s="17">
@@ -8022,7 +8453,7 @@
     </row>
     <row r="159" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B159" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="C159" s="17">
@@ -8060,7 +8491,7 @@
     </row>
     <row r="160" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B160" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="C160" s="17">
@@ -8098,7 +8529,7 @@
     </row>
     <row r="161" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B161" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="C161" s="17">
@@ -8136,7 +8567,7 @@
     </row>
     <row r="162" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B162" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="C162" s="17">
@@ -8174,7 +8605,7 @@
     </row>
     <row r="163" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B163" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="C163" s="17">
@@ -8212,7 +8643,7 @@
     </row>
     <row r="164" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B164" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="C164" s="17">
@@ -8250,7 +8681,7 @@
     </row>
     <row r="165" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B165" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="C165" s="17">
@@ -8288,7 +8719,7 @@
     </row>
     <row r="166" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B166" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="C166" s="17">
@@ -8326,7 +8757,7 @@
     </row>
     <row r="167" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B167" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="C167" s="17">
@@ -8364,7 +8795,7 @@
     </row>
     <row r="168" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B168" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="C168" s="17">
@@ -9222,7 +9653,7 @@
     </row>
     <row r="185" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B185" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="C185" s="17">
@@ -9283,7 +9714,7 @@
     </row>
     <row r="186" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B186" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="C186" s="17">
@@ -9344,7 +9775,7 @@
     </row>
     <row r="187" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B187" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="C187" s="17">
@@ -9405,7 +9836,7 @@
     </row>
     <row r="188" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B188" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="C188" s="17">
@@ -9466,7 +9897,7 @@
     </row>
     <row r="189" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B189" s="17">
-        <f t="shared" ref="B189:B213" si="2">B188+1</f>
+        <f t="shared" ref="B189:B213" si="3">B188+1</f>
         <v>76</v>
       </c>
       <c r="C189" s="17">
@@ -9527,7 +9958,7 @@
     </row>
     <row r="190" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B190" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="C190" s="17">
@@ -9588,7 +10019,7 @@
     </row>
     <row r="191" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B191" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
       <c r="C191" s="17">
@@ -9649,7 +10080,7 @@
     </row>
     <row r="192" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B192" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
       <c r="C192" s="17">
@@ -9710,7 +10141,7 @@
     </row>
     <row r="193" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B193" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="C193" s="17">
@@ -9771,7 +10202,7 @@
     </row>
     <row r="194" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B194" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="C194" s="17">
@@ -9832,7 +10263,7 @@
     </row>
     <row r="195" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B195" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="C195" s="17">
@@ -9893,7 +10324,7 @@
     </row>
     <row r="196" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B196" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83</v>
       </c>
       <c r="C196" s="17">
@@ -9954,7 +10385,7 @@
     </row>
     <row r="197" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B197" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
       <c r="C197" s="17">
@@ -10015,7 +10446,7 @@
     </row>
     <row r="198" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B198" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="C198" s="17">
@@ -10076,7 +10507,7 @@
     </row>
     <row r="199" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B199" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="C199" s="17">
@@ -10137,7 +10568,7 @@
     </row>
     <row r="200" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B200" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="C200" s="17">
@@ -10198,7 +10629,7 @@
     </row>
     <row r="201" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B201" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88</v>
       </c>
       <c r="C201" s="17">
@@ -10259,7 +10690,7 @@
     </row>
     <row r="202" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B202" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89</v>
       </c>
       <c r="C202" s="17">
@@ -10320,7 +10751,7 @@
     </row>
     <row r="203" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B203" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="C203" s="17">
@@ -10381,7 +10812,7 @@
     </row>
     <row r="204" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B204" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="C204" s="17">
@@ -10442,7 +10873,7 @@
     </row>
     <row r="205" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B205" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="C205" s="17">
@@ -10503,7 +10934,7 @@
     </row>
     <row r="206" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B206" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93</v>
       </c>
       <c r="C206" s="17">
@@ -10564,7 +10995,7 @@
     </row>
     <row r="207" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B207" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>94</v>
       </c>
       <c r="C207" s="17">
@@ -10625,7 +11056,7 @@
     </row>
     <row r="208" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B208" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>95</v>
       </c>
       <c r="C208" s="17">
@@ -10686,7 +11117,7 @@
     </row>
     <row r="209" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B209" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="C209" s="17">
@@ -10747,7 +11178,7 @@
     </row>
     <row r="210" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B210" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="C210" s="17">
@@ -10808,7 +11239,7 @@
     </row>
     <row r="211" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B211" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="C211" s="17">
@@ -10869,7 +11300,7 @@
     </row>
     <row r="212" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B212" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="C212" s="17">
@@ -10930,7 +11361,7 @@
     </row>
     <row r="213" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B213" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="C213" s="17">
@@ -11423,7 +11854,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529FEC6F-EAFA-4279-913B-5F6A84D73577}">
   <dimension ref="A1:AV222"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A69" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>